<commit_message>
SAP xls files updated
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite NI Director Prorata201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite NI Director Prorata201718.xlsx
@@ -4,53 +4,53 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="14340" windowHeight="4452" firstSheet="9" activeTab="12"/>
+    <workbookView activeTab="12" firstSheet="9" windowHeight="4452" windowWidth="14340" xWindow="384" yWindow="84"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="NIDirector_ProrataMonth1" sheetId="2" r:id="rId2"/>
-    <sheet name="PayrollForNIDirctorAsProraApril" sheetId="3" r:id="rId3"/>
-    <sheet name="TestReportsApril" sheetId="5" r:id="rId4"/>
-    <sheet name="NIDirector_ProrataMonth2" sheetId="28" r:id="rId5"/>
-    <sheet name="PayrollForNIDirctorAsProraMay" sheetId="7" r:id="rId6"/>
-    <sheet name="TestReportsMay" sheetId="6" r:id="rId7"/>
-    <sheet name="NIDirector_ProrataMonth3" sheetId="29" r:id="rId8"/>
-    <sheet name="PayrollForNIDirctorAsProraJune" sheetId="9" r:id="rId9"/>
-    <sheet name="TestReportsJune" sheetId="8" r:id="rId10"/>
-    <sheet name="NIDirector_ProrataMonth4" sheetId="30" r:id="rId11"/>
-    <sheet name="PayrollForNIDirctorAsProraJuly" sheetId="10" r:id="rId12"/>
-    <sheet name="TestReportsJuly" sheetId="19" r:id="rId13"/>
-    <sheet name="NIDirector_ProrataMonth5" sheetId="31" r:id="rId14"/>
-    <sheet name="PayrollForNIDirctorAsProraAug" sheetId="11" r:id="rId15"/>
-    <sheet name="TestReportsAugust" sheetId="20" r:id="rId16"/>
-    <sheet name="NIDirector_ProrataMonth6" sheetId="32" r:id="rId17"/>
-    <sheet name="PayrollForNIDirctorAsProraSep" sheetId="12" r:id="rId18"/>
-    <sheet name="TestReportsSeptember" sheetId="21" r:id="rId19"/>
-    <sheet name="NIDirector_ProrataMonth7" sheetId="33" r:id="rId20"/>
-    <sheet name="PayrollForNIDirctorAsProraOct" sheetId="13" r:id="rId21"/>
-    <sheet name="TestReportsOctober" sheetId="22" r:id="rId22"/>
-    <sheet name="NIDirector_ProrataMonth8" sheetId="34" r:id="rId23"/>
-    <sheet name="PayrollForNIDirctorAsProraNov" sheetId="14" r:id="rId24"/>
-    <sheet name="TestReportsNovember" sheetId="23" r:id="rId25"/>
-    <sheet name="NIDirector_ProrataMonth9" sheetId="35" r:id="rId26"/>
-    <sheet name="PayrollForNIDirctorAsProraDec" sheetId="15" r:id="rId27"/>
-    <sheet name="TestReportsDecember" sheetId="24" r:id="rId28"/>
-    <sheet name="NIDirector_ProrataMonth10" sheetId="36" r:id="rId29"/>
-    <sheet name="PayrollForNIDirctorAsProraJan" sheetId="16" r:id="rId30"/>
-    <sheet name="TestReportsJanuary" sheetId="25" r:id="rId31"/>
-    <sheet name="NIDirector_ProrataMonth11" sheetId="37" r:id="rId32"/>
-    <sheet name="PayrollForNIDirctorAsProraFeb" sheetId="17" r:id="rId33"/>
-    <sheet name="TestReportsFebruary" sheetId="26" r:id="rId34"/>
-    <sheet name="NIDirector_ProrataMonth12" sheetId="4" r:id="rId35"/>
-    <sheet name="PayrollForNIDirctorAsProraMarch" sheetId="18" r:id="rId36"/>
-    <sheet name="TestReportsMarch" sheetId="27" r:id="rId37"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="NIDirector_ProrataMonth1" r:id="rId2" sheetId="2"/>
+    <sheet name="PayrollForNIDirctorAsProraApril" r:id="rId3" sheetId="3"/>
+    <sheet name="TestReportsApril" r:id="rId4" sheetId="5"/>
+    <sheet name="NIDirector_ProrataMonth2" r:id="rId5" sheetId="28"/>
+    <sheet name="PayrollForNIDirctorAsProraMay" r:id="rId6" sheetId="7"/>
+    <sheet name="TestReportsMay" r:id="rId7" sheetId="6"/>
+    <sheet name="NIDirector_ProrataMonth3" r:id="rId8" sheetId="29"/>
+    <sheet name="PayrollForNIDirctorAsProraJune" r:id="rId9" sheetId="9"/>
+    <sheet name="TestReportsJune" r:id="rId10" sheetId="8"/>
+    <sheet name="NIDirector_ProrataMonth4" r:id="rId11" sheetId="30"/>
+    <sheet name="PayrollForNIDirctorAsProraJuly" r:id="rId12" sheetId="10"/>
+    <sheet name="TestReportsJuly" r:id="rId13" sheetId="19"/>
+    <sheet name="NIDirector_ProrataMonth5" r:id="rId14" sheetId="31"/>
+    <sheet name="PayrollForNIDirctorAsProraAug" r:id="rId15" sheetId="11"/>
+    <sheet name="TestReportsAugust" r:id="rId16" sheetId="20"/>
+    <sheet name="NIDirector_ProrataMonth6" r:id="rId17" sheetId="32"/>
+    <sheet name="PayrollForNIDirctorAsProraSep" r:id="rId18" sheetId="12"/>
+    <sheet name="TestReportsSeptember" r:id="rId19" sheetId="21"/>
+    <sheet name="NIDirector_ProrataMonth7" r:id="rId20" sheetId="33"/>
+    <sheet name="PayrollForNIDirctorAsProraOct" r:id="rId21" sheetId="13"/>
+    <sheet name="TestReportsOctober" r:id="rId22" sheetId="22"/>
+    <sheet name="NIDirector_ProrataMonth8" r:id="rId23" sheetId="34"/>
+    <sheet name="PayrollForNIDirctorAsProraNov" r:id="rId24" sheetId="14"/>
+    <sheet name="TestReportsNovember" r:id="rId25" sheetId="23"/>
+    <sheet name="NIDirector_ProrataMonth9" r:id="rId26" sheetId="35"/>
+    <sheet name="PayrollForNIDirctorAsProraDec" r:id="rId27" sheetId="15"/>
+    <sheet name="TestReportsDecember" r:id="rId28" sheetId="24"/>
+    <sheet name="NIDirector_ProrataMonth10" r:id="rId29" sheetId="36"/>
+    <sheet name="PayrollForNIDirctorAsProraJan" r:id="rId30" sheetId="16"/>
+    <sheet name="TestReportsJanuary" r:id="rId31" sheetId="25"/>
+    <sheet name="NIDirector_ProrataMonth11" r:id="rId32" sheetId="37"/>
+    <sheet name="PayrollForNIDirctorAsProraFeb" r:id="rId33" sheetId="17"/>
+    <sheet name="TestReportsFebruary" r:id="rId34" sheetId="26"/>
+    <sheet name="NIDirector_ProrataMonth12" r:id="rId35" sheetId="4"/>
+    <sheet name="PayrollForNIDirctorAsProraMarch" r:id="rId36" sheetId="18"/>
+    <sheet name="TestReportsMarch" r:id="rId37" sheetId="27"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="115">
   <si>
     <t>TC</t>
   </si>
@@ -401,6 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,52 +449,52 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -507,10 +508,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -668,7 +669,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -677,13 +678,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -693,7 +694,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -702,7 +703,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -711,7 +712,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -721,12 +722,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -757,7 +758,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -776,7 +777,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -788,7 +789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -797,10 +798,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="54.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -831,7 +832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="3" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -845,7 +846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="4" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>85</v>
       </c>
@@ -859,7 +860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="16.2" r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -873,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="6" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>74</v>
       </c>
@@ -887,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="24" r="7" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>86</v>
       </c>
@@ -901,7 +902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="19.8" r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
@@ -915,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="9" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>75</v>
       </c>
@@ -929,7 +930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="10" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>87</v>
       </c>
@@ -943,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="25.8" r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -957,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="12" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>76</v>
       </c>
@@ -971,7 +972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="13" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>88</v>
       </c>
@@ -985,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="14" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>64</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="15" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="16" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>89</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="17" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>65</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="18" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="19" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="23.4" r="20" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="21" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>79</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="22" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="24" r="23" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>67</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="24" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>80</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="25" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>92</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27" r="26" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>68</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="27" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>81</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="28" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>93</v>
       </c>
@@ -1195,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="22.8" r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>69</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="30" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>82</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="31" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>94</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="24.6" r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>70</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="33" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>83</v>
       </c>
@@ -1265,7 +1266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="34" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>95</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="24.6" r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>71</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="36" s="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="22.8" r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>72</v>
       </c>
@@ -1336,13 +1337,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1351,20 +1352,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="62.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="62.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -1451,15 +1452,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1468,14 +1469,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1504,7 +1505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -1528,12 +1529,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1542,20 +1543,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="74.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="74.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -1633,14 +1634,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1649,21 +1650,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="59.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -1747,15 +1748,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1764,16 +1765,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -1826,12 +1827,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1840,19 +1841,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="77.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="77.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -1930,14 +1931,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1946,20 +1947,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="63.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="57.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="63.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="27.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2043,15 +2044,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2060,13 +2061,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -2119,12 +2120,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2133,19 +2134,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="65.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="54.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="65.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2186,7 +2187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2223,14 +2224,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2239,21 +2240,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="65.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.77734375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="65.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2337,15 +2338,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2354,14 +2355,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.77734375" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="14.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="13.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="15.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -2415,13 +2416,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2430,15 +2431,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="36.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -2491,12 +2492,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2505,19 +2506,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="64.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="64.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2595,14 +2596,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2611,20 +2612,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="64.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="64.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2668,7 +2669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2708,15 +2709,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2725,15 +2726,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -2786,12 +2787,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2800,19 +2801,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="50" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="64.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="50.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="36.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="64.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -2890,14 +2891,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2906,20 +2907,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="67.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="45.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="67.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -2963,7 +2964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3003,15 +3004,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3020,15 +3021,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -3081,12 +3082,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3095,19 +3096,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="63.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="63.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3185,14 +3186,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3201,20 +3202,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="49.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="74.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="49.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="74.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3298,15 +3299,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3315,15 +3316,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -3376,12 +3377,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3390,19 +3391,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="42" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="63.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="63.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3480,14 +3481,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3496,19 +3497,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="41.77734375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="61.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="41.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="61.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3586,14 +3587,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3602,20 +3603,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="54.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="47.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="68.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3659,7 +3660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3699,15 +3700,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3716,15 +3717,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -3777,12 +3778,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3791,20 +3792,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="67.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="67.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3845,7 +3846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3882,14 +3883,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3898,20 +3899,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="64.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="64.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -3995,15 +3996,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId2" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4012,17 +4013,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="6.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4051,7 +4052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -4078,13 +4079,13 @@
       <c r="D4" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4093,19 +4094,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.21875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="71.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.21875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.21875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="71.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4183,14 +4184,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -4199,21 +4200,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="65.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.21875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="65.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4257,7 +4258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4297,15 +4298,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://eu2.salesforce.com/a2Qb0000000E8HTEA0" r:id="rId2" ref="C2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4314,20 +4315,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="57.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.21875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="53.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="57.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.21875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="27.6" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4411,14 +4412,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4427,15 +4428,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -4486,12 +4487,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4500,19 +4501,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.77734375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="39.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="62.21875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="62.21875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4553,7 +4554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4590,14 +4591,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -4606,21 +4607,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="65.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="51.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="65.109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="1" s="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="34.200000000000003" r="2" s="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4704,14 +4705,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4720,16 +4721,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>100</v>
       </c>
@@ -4782,13 +4783,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4797,19 +4798,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35.77734375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="65.77734375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="65.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="26.4" r="1" s="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4850,7 +4851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="36" r="2" s="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
@@ -4887,8 +4888,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://eu2.salesforce.com/a0Xb000000OaLioEAF"/>
+    <hyperlink display="https://eu2.salesforce.com/a0Xb000000OaLioEAF" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>